<commit_message>
tracks split identifiers column
</commit_message>
<xml_diff>
--- a/test_data/empty_data.xlsx
+++ b/test_data/empty_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Enclosure</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Sex</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifiers</t>
+    <t xml:space="preserve">Internal House Name</t>
   </si>
   <si>
     <t xml:space="preserve">Population _Male</t>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Population _Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag /Band</t>
   </si>
 </sst>
 </file>
@@ -180,19 +183,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,6 +252,9 @@
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -294,7 +300,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
column from tracks uses 2 spaces
report message about which columns are missing
</commit_message>
<xml_diff>
--- a/test_data/empty_data.xlsx
+++ b/test_data/empty_data.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Sex</t>
   </si>
   <si>
-    <t xml:space="preserve">Internal House Name</t>
+    <t xml:space="preserve">Internal  House  Name</t>
   </si>
   <si>
     <t xml:space="preserve">Population _Male</t>
@@ -190,10 +190,10 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.42"/>
   </cols>

</xml_diff>

<commit_message>
Tracks rem identifiers column (#171)
* black

* tracks split identifiers column

* column from tracks uses 2 spaces

report message about which columns are missing
</commit_message>
<xml_diff>
--- a/test_data/empty_data.xlsx
+++ b/test_data/empty_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Enclosure</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Sex</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifiers</t>
+    <t xml:space="preserve">Internal  House  Name</t>
   </si>
   <si>
     <t xml:space="preserve">Population _Male</t>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Population _Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag /Band</t>
   </si>
 </sst>
 </file>
@@ -180,19 +183,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,6 +252,9 @@
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -294,7 +300,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>